<commit_message>
excel file for a data structure
</commit_message>
<xml_diff>
--- a/DataStructures.xlsx
+++ b/DataStructures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Roelle\BCIT\COMP 1930 Project\Group 17 Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92102C22-E782-4368-8A61-CC8F2CCBA075}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B21102-3EE1-452F-B56A-82F6E79E11A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{B1DDA2C1-6D63-4A04-B534-F6953F098EBF}"/>
   </bookViews>
@@ -271,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -288,9 +288,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -303,11 +300,20 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -330,15 +336,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>624840</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>125730</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -384,15 +390,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>567690</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>49530</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>102870</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -438,15 +444,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>259080</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>300990</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>41910</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -790,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1557C922-CF8F-4E99-8672-BC570B207508}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="B3:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -801,219 +807,216 @@
     <col min="2" max="2" width="15.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="10" t="s">
+    <row r="3" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="4" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="D1" s="10" t="s">
+      <c r="C4" s="18"/>
+      <c r="E4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="1:10" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="2:11" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="D2" s="1" t="s">
+      <c r="C5" s="2"/>
+      <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="1" t="s">
+      <c r="F5" s="5"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="D3" s="1" t="s">
+      <c r="C6" s="2"/>
+      <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="1" t="s">
+      <c r="F6" s="5"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="D4" s="1" t="s">
+      <c r="C7" s="2"/>
+      <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A5" s="1" t="s">
+      <c r="F7" s="5"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="D5" s="7" t="s">
+      <c r="C8" s="2"/>
+      <c r="E8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="2"/>
-      <c r="I5" s="15" t="s">
+      <c r="F8" s="5"/>
+      <c r="G8" s="2"/>
+      <c r="J8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="16"/>
-    </row>
-    <row r="6" spans="1:10" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1" t="s">
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="2:11" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="D6" s="1" t="s">
+      <c r="C9" s="2"/>
+      <c r="E9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="2"/>
-      <c r="I6" s="1" t="s">
+      <c r="F9" s="5"/>
+      <c r="G9" s="2"/>
+      <c r="J9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1" t="s">
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="D7" s="1" t="s">
+      <c r="C10" s="2"/>
+      <c r="E10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="2"/>
-      <c r="I7" s="1" t="s">
+      <c r="F10" s="5"/>
+      <c r="G10" s="2"/>
+      <c r="J10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A8" s="1" t="s">
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="D8" s="1" t="s">
+      <c r="C11" s="2"/>
+      <c r="E11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="2"/>
-      <c r="I8" s="3" t="s">
+      <c r="F11" s="5"/>
+      <c r="G11" s="2"/>
+      <c r="J11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="1" t="s">
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="D9" s="10" t="s">
+      <c r="C12" s="2"/>
+      <c r="E12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="3" t="s">
+      <c r="F12" s="11"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="2:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="D10" s="9" t="s">
+      <c r="C13" s="4"/>
+      <c r="E13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="2"/>
-      <c r="I10" s="17" t="s">
+      <c r="F13" s="8"/>
+      <c r="G13" s="2"/>
+      <c r="J13" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="18"/>
-    </row>
-    <row r="11" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="D11" s="3" t="s">
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="E14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="2"/>
-      <c r="I11" s="1" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="2"/>
+      <c r="J14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="D12" s="1"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="2"/>
-      <c r="I12" s="1" t="s">
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="E15" s="1"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="2"/>
+      <c r="J15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="D13" s="10" t="s">
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="E16" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="2"/>
-      <c r="I13" s="1" t="s">
+      <c r="F16" s="11"/>
+      <c r="G16" s="2"/>
+      <c r="J16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="D14" s="6" t="s">
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="5:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="E17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="I14" s="1" t="s">
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="J17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="I15" s="1" t="s">
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="5:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="J18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="E16" s="13" t="s">
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="5:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="F19" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="14"/>
-      <c r="I16" s="1" t="s">
+      <c r="G19" s="13"/>
+      <c r="J19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="5:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="E17" s="3" t="s">
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="5:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="F20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="I17" s="1" t="s">
+      <c r="G20" s="4"/>
+      <c r="J20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="5:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="I18" s="3" t="s">
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="5:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="J21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J18" s="4"/>
+      <c r="K21" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="I10:J10"/>
+  <mergeCells count="3">
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
writing and reading data
</commit_message>
<xml_diff>
--- a/DataStructures.xlsx
+++ b/DataStructures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Roelle\BCIT\COMP 1930 Project\Group 17 Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B21102-3EE1-452F-B56A-82F6E79E11A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D025EC50-F777-4819-82C4-6B62C6EED95D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{B1DDA2C1-6D63-4A04-B534-F6953F098EBF}"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8994" xr2:uid="{B1DDA2C1-6D63-4A04-B534-F6953F098EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -300,6 +300,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -308,12 +314,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1557C922-CF8F-4E99-8672-BC570B207508}">
   <dimension ref="B3:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -809,15 +809,15 @@
   <sheetData>
     <row r="3" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="4" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="E4" s="16" t="s">
+      <c r="C4" s="20"/>
+      <c r="E4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
     </row>
     <row r="5" spans="2:11" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="1" t="s">
@@ -933,10 +933,10 @@
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="2"/>
-      <c r="J13" s="19" t="s">
+      <c r="J13" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="K13" s="20"/>
+      <c r="K13" s="17"/>
     </row>
     <row r="14" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="E14" s="3" t="s">

</xml_diff>

<commit_message>
pop up event details
</commit_message>
<xml_diff>
--- a/DataStructures.xlsx
+++ b/DataStructures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Roelle\BCIT\COMP 1930 Project\Group 17 Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D025EC50-F777-4819-82C4-6B62C6EED95D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A53CFC-E1E9-40F9-BC36-3312D2AB4A49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8994" xr2:uid="{B1DDA2C1-6D63-4A04-B534-F6953F098EBF}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{B1DDA2C1-6D63-4A04-B534-F6953F098EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>User</t>
   </si>
@@ -63,33 +63,15 @@
     <t>profile picture</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>Skill level</t>
   </si>
   <si>
     <t># of people</t>
   </si>
   <si>
-    <t>Message</t>
-  </si>
-  <si>
     <t>Events</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>Guests</t>
-  </si>
-  <si>
     <t>beginner</t>
   </si>
   <si>
@@ -133,6 +115,30 @@
   </si>
   <si>
     <t>Position</t>
+  </si>
+  <si>
+    <t>host</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>skill level</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Keep first letter lowercase for database</t>
   </si>
 </sst>
 </file>
@@ -799,7 +805,7 @@
   <dimension ref="B3:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -807,14 +813,18 @@
     <col min="2" max="2" width="15.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="3" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="4" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B4" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="20"/>
       <c r="E4" s="18" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -825,7 +835,7 @@
       </c>
       <c r="C5" s="2"/>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="2"/>
@@ -836,7 +846,7 @@
       </c>
       <c r="C6" s="2"/>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="2"/>
@@ -847,7 +857,7 @@
       </c>
       <c r="C7" s="2"/>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="2"/>
@@ -858,12 +868,12 @@
       </c>
       <c r="C8" s="2"/>
       <c r="E8" s="7" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="2"/>
       <c r="J8" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="K8" s="15"/>
     </row>
@@ -873,12 +883,12 @@
       </c>
       <c r="C9" s="2"/>
       <c r="E9" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="2"/>
       <c r="J9" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="K9" s="2"/>
     </row>
@@ -888,12 +898,12 @@
       </c>
       <c r="C10" s="2"/>
       <c r="E10" s="1" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="2"/>
       <c r="J10" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="K10" s="2"/>
     </row>
@@ -903,12 +913,12 @@
       </c>
       <c r="C11" s="2"/>
       <c r="E11" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="2"/>
       <c r="J11" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="K11" s="4"/>
     </row>
@@ -918,7 +928,7 @@
       </c>
       <c r="C12" s="2"/>
       <c r="E12" s="10" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="2"/>
@@ -929,23 +939,23 @@
       </c>
       <c r="C13" s="4"/>
       <c r="E13" s="9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="2"/>
       <c r="J13" s="16" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="K13" s="17"/>
     </row>
     <row r="14" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="E14" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="2"/>
       <c r="J14" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="K14" s="2"/>
     </row>
@@ -954,61 +964,61 @@
       <c r="F15" s="5"/>
       <c r="G15" s="2"/>
       <c r="J15" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="2:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="E16" s="10" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="2"/>
       <c r="J16" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="5:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="E17" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="J17" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="5:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="J18" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="5:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="F19" s="12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G19" s="13"/>
       <c r="J19" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="5:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="F20" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G20" s="4"/>
       <c r="J20" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="5:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="J21" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K21" s="4"/>
     </row>

</xml_diff>